<commit_message>
Bug fixed: dynamic start and end times
</commit_message>
<xml_diff>
--- a/schedule3.xlsx
+++ b/schedule3.xlsx
@@ -467,7 +467,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AI12"/>
+  <dimension ref="A1:AE12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -506,10 +506,6 @@
     <col width="6" customWidth="1" min="29" max="29"/>
     <col width="6" customWidth="1" min="30" max="30"/>
     <col width="6" customWidth="1" min="31" max="31"/>
-    <col width="6" customWidth="1" min="32" max="32"/>
-    <col width="6" customWidth="1" min="33" max="33"/>
-    <col width="6" customWidth="1" min="34" max="34"/>
-    <col width="6" customWidth="1" min="35" max="35"/>
   </cols>
   <sheetData>
     <row r="1" ht="20" customHeight="1">
@@ -520,170 +516,150 @@
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>11:00</t>
+          <t>12:00</t>
         </is>
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>11:15</t>
+          <t>12:15</t>
         </is>
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>11:30</t>
+          <t>12:30</t>
         </is>
       </c>
       <c r="E1" s="1" t="inlineStr">
         <is>
-          <t>11:45</t>
+          <t>12:45</t>
         </is>
       </c>
       <c r="F1" s="1" t="inlineStr">
         <is>
-          <t>12:00</t>
+          <t>13:00</t>
         </is>
       </c>
       <c r="G1" s="1" t="inlineStr">
         <is>
-          <t>12:15</t>
+          <t>13:15</t>
         </is>
       </c>
       <c r="H1" s="1" t="inlineStr">
         <is>
-          <t>12:30</t>
+          <t>13:30</t>
         </is>
       </c>
       <c r="I1" s="1" t="inlineStr">
         <is>
-          <t>12:45</t>
+          <t>13:45</t>
         </is>
       </c>
       <c r="J1" s="1" t="inlineStr">
         <is>
-          <t>13:00</t>
+          <t>14:00</t>
         </is>
       </c>
       <c r="K1" s="1" t="inlineStr">
         <is>
-          <t>13:15</t>
+          <t>14:15</t>
         </is>
       </c>
       <c r="L1" s="1" t="inlineStr">
         <is>
-          <t>13:30</t>
+          <t>14:30</t>
         </is>
       </c>
       <c r="M1" s="1" t="inlineStr">
         <is>
-          <t>13:45</t>
+          <t>14:45</t>
         </is>
       </c>
       <c r="N1" s="1" t="inlineStr">
         <is>
-          <t>14:00</t>
+          <t>15:00</t>
         </is>
       </c>
       <c r="O1" s="1" t="inlineStr">
         <is>
-          <t>14:15</t>
+          <t>15:15</t>
         </is>
       </c>
       <c r="P1" s="1" t="inlineStr">
         <is>
-          <t>14:30</t>
+          <t>15:30</t>
         </is>
       </c>
       <c r="Q1" s="1" t="inlineStr">
         <is>
-          <t>14:45</t>
+          <t>15:45</t>
         </is>
       </c>
       <c r="R1" s="1" t="inlineStr">
         <is>
-          <t>15:00</t>
+          <t>16:00</t>
         </is>
       </c>
       <c r="S1" s="1" t="inlineStr">
         <is>
-          <t>15:15</t>
+          <t>16:15</t>
         </is>
       </c>
       <c r="T1" s="1" t="inlineStr">
         <is>
-          <t>15:30</t>
+          <t>16:30</t>
         </is>
       </c>
       <c r="U1" s="1" t="inlineStr">
         <is>
-          <t>15:45</t>
+          <t>16:45</t>
         </is>
       </c>
       <c r="V1" s="1" t="inlineStr">
         <is>
-          <t>16:00</t>
+          <t>17:00</t>
         </is>
       </c>
       <c r="W1" s="1" t="inlineStr">
         <is>
-          <t>16:15</t>
+          <t>17:15</t>
         </is>
       </c>
       <c r="X1" s="1" t="inlineStr">
         <is>
-          <t>16:30</t>
+          <t>17:30</t>
         </is>
       </c>
       <c r="Y1" s="1" t="inlineStr">
         <is>
-          <t>16:45</t>
+          <t>17:45</t>
         </is>
       </c>
       <c r="Z1" s="1" t="inlineStr">
         <is>
-          <t>17:00</t>
+          <t>18:00</t>
         </is>
       </c>
       <c r="AA1" s="1" t="inlineStr">
         <is>
-          <t>17:15</t>
+          <t>18:15</t>
         </is>
       </c>
       <c r="AB1" s="1" t="inlineStr">
         <is>
-          <t>17:30</t>
+          <t>18:30</t>
         </is>
       </c>
       <c r="AC1" s="1" t="inlineStr">
         <is>
-          <t>17:45</t>
+          <t>18:45</t>
         </is>
       </c>
       <c r="AD1" s="1" t="inlineStr">
         <is>
-          <t>18:00</t>
+          <t>19:00</t>
         </is>
       </c>
       <c r="AE1" s="1" t="inlineStr">
-        <is>
-          <t>18:15</t>
-        </is>
-      </c>
-      <c r="AF1" s="1" t="inlineStr">
-        <is>
-          <t>18:30</t>
-        </is>
-      </c>
-      <c r="AG1" s="1" t="inlineStr">
-        <is>
-          <t>18:45</t>
-        </is>
-      </c>
-      <c r="AH1" s="1" t="inlineStr">
-        <is>
-          <t>19:00</t>
-        </is>
-      </c>
-      <c r="AI1" s="1" t="inlineStr">
         <is>
           <t>19:15</t>
         </is>
@@ -703,72 +679,68 @@
       <c r="G2" s="3" t="inlineStr"/>
       <c r="H2" s="3" t="inlineStr"/>
       <c r="I2" s="3" t="inlineStr"/>
-      <c r="J2" s="3" t="inlineStr"/>
-      <c r="K2" s="3" t="inlineStr"/>
-      <c r="L2" s="3" t="inlineStr"/>
-      <c r="M2" s="3" t="inlineStr"/>
+      <c r="J2" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="K2" s="3" t="n">
+        <v>5</v>
+      </c>
+      <c r="L2" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="M2" s="3" t="n">
+        <v>4</v>
+      </c>
       <c r="N2" s="3" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="O2" s="3" t="n">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="P2" s="3" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="Q2" s="3" t="n">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="R2" s="3" t="n">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="S2" s="3" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="T2" s="3" t="n">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="U2" s="3" t="n">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="V2" s="3" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="W2" s="3" t="n">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="X2" s="3" t="n">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="Y2" s="3" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="Z2" s="3" t="n">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="AA2" s="3" t="n">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="AB2" s="3" t="n">
-        <v>4</v>
-      </c>
-      <c r="AC2" s="3" t="n">
-        <v>7</v>
-      </c>
-      <c r="AD2" s="3" t="n">
-        <v>3</v>
-      </c>
-      <c r="AE2" s="3" t="n">
-        <v>2</v>
-      </c>
-      <c r="AF2" s="3" t="n">
-        <v>6</v>
-      </c>
-      <c r="AG2" s="4" t="n">
-        <v>5</v>
-      </c>
-      <c r="AH2" s="3" t="inlineStr"/>
-      <c r="AI2" s="3" t="inlineStr"/>
+        <v>6</v>
+      </c>
+      <c r="AC2" s="4" t="n">
+        <v>5</v>
+      </c>
+      <c r="AD2" s="3" t="inlineStr"/>
+      <c r="AE2" s="3" t="inlineStr"/>
     </row>
     <row r="3" ht="20" customHeight="1">
       <c r="A3" s="2" t="inlineStr">
@@ -780,87 +752,83 @@
       <c r="C3" s="3" t="inlineStr"/>
       <c r="D3" s="3" t="inlineStr"/>
       <c r="E3" s="3" t="inlineStr"/>
-      <c r="F3" s="3" t="inlineStr"/>
-      <c r="G3" s="3" t="inlineStr"/>
-      <c r="H3" s="3" t="inlineStr"/>
-      <c r="I3" s="3" t="inlineStr"/>
+      <c r="F3" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="G3" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="H3" s="3" t="n">
+        <v>2</v>
+      </c>
+      <c r="I3" s="3" t="n">
+        <v>3</v>
+      </c>
       <c r="J3" s="3" t="n">
+        <v>6</v>
+      </c>
+      <c r="K3" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="L3" s="3" t="n">
+        <v>5</v>
+      </c>
+      <c r="M3" s="3" t="n">
         <v>1</v>
       </c>
-      <c r="K3" s="3" t="n">
-        <v>2</v>
-      </c>
-      <c r="L3" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="M3" s="3" t="n">
-        <v>3</v>
-      </c>
       <c r="N3" s="3" t="n">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="O3" s="3" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="P3" s="3" t="n">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="Q3" s="3" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="R3" s="3" t="n">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="S3" s="3" t="n">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="T3" s="3" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="U3" s="3" t="n">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="V3" s="3" t="n">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="W3" s="3" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="X3" s="3" t="n">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="Y3" s="3" t="n">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="Z3" s="3" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="AA3" s="3" t="n">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="AB3" s="3" t="n">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="AC3" s="3" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="AD3" s="3" t="n">
         <v>7</v>
       </c>
       <c r="AE3" s="3" t="n">
-        <v>3</v>
-      </c>
-      <c r="AF3" s="3" t="n">
-        <v>2</v>
-      </c>
-      <c r="AG3" s="3" t="n">
-        <v>6</v>
-      </c>
-      <c r="AH3" s="3" t="n">
-        <v>4</v>
-      </c>
-      <c r="AI3" s="3" t="n">
-        <v>7</v>
+        <v>4</v>
       </c>
     </row>
     <row r="4" ht="20" customHeight="1">
@@ -882,94 +850,82 @@
         <v>2</v>
       </c>
       <c r="F4" s="3" t="n">
+        <v>3</v>
+      </c>
+      <c r="G4" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="G4" s="3" t="n">
+      <c r="H4" s="3" t="n">
         <v>1</v>
       </c>
-      <c r="H4" s="3" t="n">
-        <v>2</v>
-      </c>
       <c r="I4" s="3" t="n">
+        <v>2</v>
+      </c>
+      <c r="J4" s="3" t="n">
+        <v>3</v>
+      </c>
+      <c r="K4" s="3" t="n">
+        <v>6</v>
+      </c>
+      <c r="L4" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="J4" s="3" t="n">
-        <v>3</v>
-      </c>
-      <c r="K4" s="3" t="n">
+      <c r="M4" s="3" t="n">
+        <v>5</v>
+      </c>
+      <c r="N4" s="3" t="n">
         <v>1</v>
       </c>
-      <c r="L4" s="3" t="n">
-        <v>2</v>
-      </c>
-      <c r="M4" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="N4" s="3" t="n">
-        <v>3</v>
-      </c>
       <c r="O4" s="3" t="n">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="P4" s="3" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="Q4" s="3" t="n">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="R4" s="3" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="S4" s="3" t="n">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="T4" s="3" t="n">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="U4" s="3" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="V4" s="3" t="n">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="W4" s="3" t="n">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="X4" s="3" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="Y4" s="3" t="n">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="Z4" s="3" t="n">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="AA4" s="3" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="AB4" s="3" t="n">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="AC4" s="3" t="n">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="AD4" s="3" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="AE4" s="3" t="n">
         <v>7</v>
-      </c>
-      <c r="AF4" s="3" t="n">
-        <v>3</v>
-      </c>
-      <c r="AG4" s="3" t="n">
-        <v>2</v>
-      </c>
-      <c r="AH4" s="3" t="n">
-        <v>6</v>
-      </c>
-      <c r="AI4" s="3" t="n">
-        <v>4</v>
       </c>
     </row>
     <row r="5" ht="20" customHeight="1">
@@ -994,90 +950,78 @@
         <v>2</v>
       </c>
       <c r="G5" s="3" t="n">
+        <v>3</v>
+      </c>
+      <c r="H5" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="H5" s="3" t="n">
+      <c r="I5" s="3" t="n">
         <v>1</v>
       </c>
-      <c r="I5" s="3" t="n">
-        <v>2</v>
-      </c>
       <c r="J5" s="3" t="n">
+        <v>4</v>
+      </c>
+      <c r="K5" s="3" t="n">
+        <v>3</v>
+      </c>
+      <c r="L5" s="3" t="n">
+        <v>6</v>
+      </c>
+      <c r="M5" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="K5" s="3" t="n">
-        <v>3</v>
-      </c>
-      <c r="L5" s="3" t="n">
+      <c r="N5" s="3" t="n">
+        <v>5</v>
+      </c>
+      <c r="O5" s="3" t="n">
         <v>1</v>
       </c>
-      <c r="M5" s="3" t="n">
-        <v>2</v>
-      </c>
-      <c r="N5" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="O5" s="3" t="n">
-        <v>3</v>
-      </c>
       <c r="P5" s="3" t="n">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="Q5" s="3" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="R5" s="3" t="n">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="S5" s="3" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="T5" s="3" t="n">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="U5" s="3" t="n">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="V5" s="3" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="W5" s="3" t="n">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="X5" s="3" t="n">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="Y5" s="3" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="Z5" s="3" t="n">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="AA5" s="3" t="n">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="AB5" s="3" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="AC5" s="3" t="n">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="AD5" s="3" t="n">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="AE5" s="3" t="n">
-        <v>4</v>
-      </c>
-      <c r="AF5" s="3" t="n">
-        <v>7</v>
-      </c>
-      <c r="AG5" s="3" t="n">
-        <v>3</v>
-      </c>
-      <c r="AH5" s="3" t="n">
-        <v>2</v>
-      </c>
-      <c r="AI5" s="3" t="n">
         <v>6</v>
       </c>
     </row>
@@ -1095,74 +1039,70 @@
       <c r="G6" s="3" t="inlineStr"/>
       <c r="H6" s="3" t="inlineStr"/>
       <c r="I6" s="3" t="inlineStr"/>
-      <c r="J6" s="3" t="inlineStr"/>
-      <c r="K6" s="3" t="inlineStr"/>
-      <c r="L6" s="3" t="inlineStr"/>
-      <c r="M6" s="3" t="inlineStr"/>
+      <c r="J6" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="K6" s="3" t="n">
+        <v>4</v>
+      </c>
+      <c r="L6" s="3" t="n">
+        <v>3</v>
+      </c>
+      <c r="M6" s="3" t="n">
+        <v>6</v>
+      </c>
       <c r="N6" s="3" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="O6" s="3" t="n">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="P6" s="3" t="n">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="Q6" s="3" t="n">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="R6" s="3" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="S6" s="3" t="n">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="T6" s="3" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="U6" s="3" t="n">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="V6" s="3" t="n">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="W6" s="3" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="X6" s="3" t="n">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="Y6" s="3" t="n">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="Z6" s="3" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="AA6" s="3" t="n">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="AB6" s="3" t="n">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="AC6" s="3" t="n">
-        <v>2</v>
-      </c>
-      <c r="AD6" s="3" t="n">
-        <v>6</v>
+        <v>4</v>
+      </c>
+      <c r="AD6" s="4" t="n">
+        <v>5</v>
       </c>
       <c r="AE6" s="3" t="n">
-        <v>5</v>
-      </c>
-      <c r="AF6" s="3" t="n">
-        <v>4</v>
-      </c>
-      <c r="AG6" s="3" t="n">
-        <v>7</v>
-      </c>
-      <c r="AH6" s="4" t="n">
-        <v>5</v>
-      </c>
-      <c r="AI6" s="3" t="n">
         <v>2</v>
       </c>
     </row>
@@ -1184,16 +1124,16 @@
       <c r="K7" s="3" t="inlineStr"/>
       <c r="L7" s="3" t="inlineStr"/>
       <c r="M7" s="3" t="inlineStr"/>
-      <c r="N7" s="3" t="inlineStr"/>
-      <c r="O7" s="3" t="inlineStr"/>
+      <c r="N7" s="3" t="n">
+        <v>6</v>
+      </c>
+      <c r="O7" s="3" t="n">
+        <v>0</v>
+      </c>
       <c r="P7" s="3" t="inlineStr"/>
       <c r="Q7" s="3" t="inlineStr"/>
-      <c r="R7" s="3" t="n">
-        <v>6</v>
-      </c>
-      <c r="S7" s="3" t="n">
-        <v>1</v>
-      </c>
+      <c r="R7" s="3" t="inlineStr"/>
+      <c r="S7" s="3" t="inlineStr"/>
       <c r="T7" s="3" t="inlineStr"/>
       <c r="U7" s="3" t="inlineStr"/>
       <c r="V7" s="3" t="inlineStr"/>
@@ -1206,10 +1146,6 @@
       <c r="AC7" s="3" t="inlineStr"/>
       <c r="AD7" s="3" t="inlineStr"/>
       <c r="AE7" s="3" t="inlineStr"/>
-      <c r="AF7" s="3" t="inlineStr"/>
-      <c r="AG7" s="3" t="inlineStr"/>
-      <c r="AH7" s="3" t="inlineStr"/>
-      <c r="AI7" s="3" t="inlineStr"/>
     </row>
     <row r="8" ht="20" customHeight="1">
       <c r="A8" s="2" t="inlineStr">
@@ -1247,10 +1183,6 @@
       <c r="AC8" s="3" t="inlineStr"/>
       <c r="AD8" s="3" t="inlineStr"/>
       <c r="AE8" s="3" t="inlineStr"/>
-      <c r="AF8" s="3" t="inlineStr"/>
-      <c r="AG8" s="3" t="inlineStr"/>
-      <c r="AH8" s="3" t="inlineStr"/>
-      <c r="AI8" s="3" t="inlineStr"/>
     </row>
     <row r="9" ht="20" customHeight="1">
       <c r="A9" s="2" t="inlineStr">
@@ -1288,10 +1220,6 @@
       <c r="AC9" s="3" t="inlineStr"/>
       <c r="AD9" s="3" t="inlineStr"/>
       <c r="AE9" s="3" t="inlineStr"/>
-      <c r="AF9" s="3" t="inlineStr"/>
-      <c r="AG9" s="3" t="inlineStr"/>
-      <c r="AH9" s="3" t="inlineStr"/>
-      <c r="AI9" s="3" t="inlineStr"/>
     </row>
     <row r="10" ht="20" customHeight="1">
       <c r="A10" s="2" t="inlineStr">
@@ -1318,87 +1246,75 @@
         <v>2</v>
       </c>
       <c r="H10" s="3" t="n">
+        <v>3</v>
+      </c>
+      <c r="I10" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="I10" s="3" t="n">
+      <c r="J10" s="3" t="n">
+        <v>5</v>
+      </c>
+      <c r="K10" s="3" t="n">
         <v>1</v>
       </c>
-      <c r="J10" s="3" t="n">
-        <v>2</v>
-      </c>
-      <c r="K10" s="3" t="n">
-        <v>0</v>
-      </c>
       <c r="L10" s="3" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="M10" s="3" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="N10" s="3" t="n">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="O10" s="3" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="P10" s="3" t="n">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="Q10" s="3" t="n">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="R10" s="3" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="S10" s="3" t="n">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="T10" s="3" t="n">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="U10" s="3" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="V10" s="3" t="n">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="W10" s="3" t="n">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="X10" s="3" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="Y10" s="3" t="n">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="Z10" s="3" t="n">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="AA10" s="3" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="AB10" s="3" t="n">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="AC10" s="3" t="n">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="AD10" s="3" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="AE10" s="3" t="n">
-        <v>6</v>
-      </c>
-      <c r="AF10" s="3" t="n">
-        <v>5</v>
-      </c>
-      <c r="AG10" s="3" t="n">
-        <v>4</v>
-      </c>
-      <c r="AH10" s="3" t="n">
-        <v>7</v>
-      </c>
-      <c r="AI10" s="3" t="n">
         <v>5</v>
       </c>
     </row>
@@ -1438,10 +1354,6 @@
       <c r="AC11" s="3" t="inlineStr"/>
       <c r="AD11" s="3" t="inlineStr"/>
       <c r="AE11" s="3" t="inlineStr"/>
-      <c r="AF11" s="3" t="inlineStr"/>
-      <c r="AG11" s="3" t="inlineStr"/>
-      <c r="AH11" s="3" t="inlineStr"/>
-      <c r="AI11" s="3" t="inlineStr"/>
     </row>
     <row r="12" ht="20" customHeight="1">
       <c r="A12" s="2" t="inlineStr">
@@ -1479,10 +1391,6 @@
       <c r="AC12" s="3" t="inlineStr"/>
       <c r="AD12" s="3" t="inlineStr"/>
       <c r="AE12" s="3" t="inlineStr"/>
-      <c r="AF12" s="3" t="inlineStr"/>
-      <c r="AG12" s="3" t="inlineStr"/>
-      <c r="AH12" s="3" t="inlineStr"/>
-      <c r="AI12" s="3" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Bug fixed: multiple shifts in one day
</commit_message>
<xml_diff>
--- a/schedule3.xlsx
+++ b/schedule3.xlsx
@@ -38,7 +38,7 @@
       <sz val="10"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="5">
     <fill>
       <patternFill/>
     </fill>
@@ -63,12 +63,6 @@
         <bgColor rgb="00FFFFFF"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="00CCCCCC"/>
-        <bgColor rgb="00CCCCCC"/>
-      </patternFill>
-    </fill>
   </fills>
   <borders count="2">
     <border>
@@ -88,7 +82,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
@@ -97,9 +91,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -467,7 +458,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AE12"/>
+  <dimension ref="A1:AI12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -506,6 +497,10 @@
     <col width="6" customWidth="1" min="29" max="29"/>
     <col width="6" customWidth="1" min="30" max="30"/>
     <col width="6" customWidth="1" min="31" max="31"/>
+    <col width="6" customWidth="1" min="32" max="32"/>
+    <col width="6" customWidth="1" min="33" max="33"/>
+    <col width="6" customWidth="1" min="34" max="34"/>
+    <col width="6" customWidth="1" min="35" max="35"/>
   </cols>
   <sheetData>
     <row r="1" ht="20" customHeight="1">
@@ -516,150 +511,170 @@
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
+          <t>11:00</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>11:15</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>11:30</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>11:45</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
           <t>12:00</t>
         </is>
       </c>
-      <c r="C1" s="1" t="inlineStr">
+      <c r="G1" s="1" t="inlineStr">
         <is>
           <t>12:15</t>
         </is>
       </c>
-      <c r="D1" s="1" t="inlineStr">
+      <c r="H1" s="1" t="inlineStr">
         <is>
           <t>12:30</t>
         </is>
       </c>
-      <c r="E1" s="1" t="inlineStr">
+      <c r="I1" s="1" t="inlineStr">
         <is>
           <t>12:45</t>
         </is>
       </c>
-      <c r="F1" s="1" t="inlineStr">
+      <c r="J1" s="1" t="inlineStr">
         <is>
           <t>13:00</t>
         </is>
       </c>
-      <c r="G1" s="1" t="inlineStr">
+      <c r="K1" s="1" t="inlineStr">
         <is>
           <t>13:15</t>
         </is>
       </c>
-      <c r="H1" s="1" t="inlineStr">
+      <c r="L1" s="1" t="inlineStr">
         <is>
           <t>13:30</t>
         </is>
       </c>
-      <c r="I1" s="1" t="inlineStr">
+      <c r="M1" s="1" t="inlineStr">
         <is>
           <t>13:45</t>
         </is>
       </c>
-      <c r="J1" s="1" t="inlineStr">
+      <c r="N1" s="1" t="inlineStr">
         <is>
           <t>14:00</t>
         </is>
       </c>
-      <c r="K1" s="1" t="inlineStr">
+      <c r="O1" s="1" t="inlineStr">
         <is>
           <t>14:15</t>
         </is>
       </c>
-      <c r="L1" s="1" t="inlineStr">
+      <c r="P1" s="1" t="inlineStr">
         <is>
           <t>14:30</t>
         </is>
       </c>
-      <c r="M1" s="1" t="inlineStr">
+      <c r="Q1" s="1" t="inlineStr">
         <is>
           <t>14:45</t>
         </is>
       </c>
-      <c r="N1" s="1" t="inlineStr">
+      <c r="R1" s="1" t="inlineStr">
         <is>
           <t>15:00</t>
         </is>
       </c>
-      <c r="O1" s="1" t="inlineStr">
+      <c r="S1" s="1" t="inlineStr">
         <is>
           <t>15:15</t>
         </is>
       </c>
-      <c r="P1" s="1" t="inlineStr">
+      <c r="T1" s="1" t="inlineStr">
         <is>
           <t>15:30</t>
         </is>
       </c>
-      <c r="Q1" s="1" t="inlineStr">
+      <c r="U1" s="1" t="inlineStr">
         <is>
           <t>15:45</t>
         </is>
       </c>
-      <c r="R1" s="1" t="inlineStr">
+      <c r="V1" s="1" t="inlineStr">
         <is>
           <t>16:00</t>
         </is>
       </c>
-      <c r="S1" s="1" t="inlineStr">
+      <c r="W1" s="1" t="inlineStr">
         <is>
           <t>16:15</t>
         </is>
       </c>
-      <c r="T1" s="1" t="inlineStr">
+      <c r="X1" s="1" t="inlineStr">
         <is>
           <t>16:30</t>
         </is>
       </c>
-      <c r="U1" s="1" t="inlineStr">
+      <c r="Y1" s="1" t="inlineStr">
         <is>
           <t>16:45</t>
         </is>
       </c>
-      <c r="V1" s="1" t="inlineStr">
+      <c r="Z1" s="1" t="inlineStr">
         <is>
           <t>17:00</t>
         </is>
       </c>
-      <c r="W1" s="1" t="inlineStr">
+      <c r="AA1" s="1" t="inlineStr">
         <is>
           <t>17:15</t>
         </is>
       </c>
-      <c r="X1" s="1" t="inlineStr">
+      <c r="AB1" s="1" t="inlineStr">
         <is>
           <t>17:30</t>
         </is>
       </c>
-      <c r="Y1" s="1" t="inlineStr">
+      <c r="AC1" s="1" t="inlineStr">
         <is>
           <t>17:45</t>
         </is>
       </c>
-      <c r="Z1" s="1" t="inlineStr">
+      <c r="AD1" s="1" t="inlineStr">
         <is>
           <t>18:00</t>
         </is>
       </c>
-      <c r="AA1" s="1" t="inlineStr">
+      <c r="AE1" s="1" t="inlineStr">
         <is>
           <t>18:15</t>
         </is>
       </c>
-      <c r="AB1" s="1" t="inlineStr">
+      <c r="AF1" s="1" t="inlineStr">
         <is>
           <t>18:30</t>
         </is>
       </c>
-      <c r="AC1" s="1" t="inlineStr">
+      <c r="AG1" s="1" t="inlineStr">
         <is>
           <t>18:45</t>
         </is>
       </c>
-      <c r="AD1" s="1" t="inlineStr">
+      <c r="AH1" s="1" t="inlineStr">
         <is>
           <t>19:00</t>
         </is>
       </c>
-      <c r="AE1" s="1" t="inlineStr">
+      <c r="AI1" s="1" t="inlineStr">
         <is>
           <t>19:15</t>
         </is>
@@ -671,76 +686,108 @@
           <t>Kiddie</t>
         </is>
       </c>
-      <c r="B2" s="3" t="inlineStr"/>
-      <c r="C2" s="3" t="inlineStr"/>
-      <c r="D2" s="3" t="inlineStr"/>
-      <c r="E2" s="3" t="inlineStr"/>
-      <c r="F2" s="3" t="inlineStr"/>
-      <c r="G2" s="3" t="inlineStr"/>
-      <c r="H2" s="3" t="inlineStr"/>
-      <c r="I2" s="3" t="inlineStr"/>
+      <c r="B2" s="3" t="n">
+        <v>2</v>
+      </c>
+      <c r="C2" s="3" t="n">
+        <v>6</v>
+      </c>
+      <c r="D2" s="3" t="n">
+        <v>4</v>
+      </c>
+      <c r="E2" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="F2" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="G2" s="3" t="n">
+        <v>3</v>
+      </c>
+      <c r="H2" s="3" t="n">
+        <v>5</v>
+      </c>
+      <c r="I2" s="3" t="n">
+        <v>2</v>
+      </c>
       <c r="J2" s="3" t="n">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="K2" s="3" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="L2" s="3" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="M2" s="3" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="N2" s="3" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="O2" s="3" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="P2" s="3" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="Q2" s="3" t="n">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="R2" s="3" t="n">
         <v>7</v>
       </c>
       <c r="S2" s="3" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="T2" s="3" t="n">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="U2" s="3" t="n">
-        <v>2</v>
+        <v>9</v>
       </c>
       <c r="V2" s="3" t="n">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="W2" s="3" t="n">
         <v>5</v>
       </c>
       <c r="X2" s="3" t="n">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="Y2" s="3" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="Z2" s="3" t="n">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="AA2" s="3" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="AB2" s="3" t="n">
-        <v>6</v>
-      </c>
-      <c r="AC2" s="4" t="n">
-        <v>5</v>
-      </c>
-      <c r="AD2" s="3" t="inlineStr"/>
-      <c r="AE2" s="3" t="inlineStr"/>
+        <v>8</v>
+      </c>
+      <c r="AC2" s="3" t="n">
+        <v>9</v>
+      </c>
+      <c r="AD2" s="3" t="n">
+        <v>10</v>
+      </c>
+      <c r="AE2" s="3" t="n">
+        <v>5</v>
+      </c>
+      <c r="AF2" s="3" t="n">
+        <v>4</v>
+      </c>
+      <c r="AG2" s="3" t="n">
+        <v>6</v>
+      </c>
+      <c r="AH2" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="AI2" s="3" t="n">
+        <v>8</v>
+      </c>
     </row>
     <row r="3" ht="20" customHeight="1">
       <c r="A3" s="2" t="inlineStr">
@@ -748,10 +795,18 @@
           <t>Dive</t>
         </is>
       </c>
-      <c r="B3" s="3" t="inlineStr"/>
-      <c r="C3" s="3" t="inlineStr"/>
-      <c r="D3" s="3" t="inlineStr"/>
-      <c r="E3" s="3" t="inlineStr"/>
+      <c r="B3" s="3" t="n">
+        <v>5</v>
+      </c>
+      <c r="C3" s="3" t="n">
+        <v>2</v>
+      </c>
+      <c r="D3" s="3" t="n">
+        <v>6</v>
+      </c>
+      <c r="E3" s="3" t="n">
+        <v>4</v>
+      </c>
       <c r="F3" s="3" t="n">
         <v>0</v>
       </c>
@@ -759,76 +814,88 @@
         <v>1</v>
       </c>
       <c r="H3" s="3" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="I3" s="3" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="J3" s="3" t="n">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="K3" s="3" t="n">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="L3" s="3" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="M3" s="3" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="N3" s="3" t="n">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="O3" s="3" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="P3" s="3" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="Q3" s="3" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="R3" s="3" t="n">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="S3" s="3" t="n">
         <v>7</v>
       </c>
       <c r="T3" s="3" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="U3" s="3" t="n">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="V3" s="3" t="n">
-        <v>2</v>
+        <v>9</v>
       </c>
       <c r="W3" s="3" t="n">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="X3" s="3" t="n">
         <v>5</v>
       </c>
       <c r="Y3" s="3" t="n">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="Z3" s="3" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="AA3" s="3" t="n">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="AB3" s="3" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="AC3" s="3" t="n">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="AD3" s="3" t="n">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="AE3" s="3" t="n">
-        <v>4</v>
+        <v>10</v>
+      </c>
+      <c r="AF3" s="3" t="n">
+        <v>5</v>
+      </c>
+      <c r="AG3" s="3" t="n">
+        <v>4</v>
+      </c>
+      <c r="AH3" s="3" t="n">
+        <v>6</v>
+      </c>
+      <c r="AI3" s="3" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="4" ht="20" customHeight="1">
@@ -838,19 +905,19 @@
         </is>
       </c>
       <c r="B4" s="3" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C4" s="3" t="n">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="D4" s="3" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E4" s="3" t="n">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="F4" s="3" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="G4" s="3" t="n">
         <v>0</v>
@@ -859,73 +926,85 @@
         <v>1</v>
       </c>
       <c r="I4" s="3" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="J4" s="3" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="K4" s="3" t="n">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="L4" s="3" t="n">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="M4" s="3" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="N4" s="3" t="n">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="O4" s="3" t="n">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="P4" s="3" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="Q4" s="3" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="R4" s="3" t="n">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="S4" s="3" t="n">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="T4" s="3" t="n">
         <v>7</v>
       </c>
       <c r="U4" s="3" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="V4" s="3" t="n">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="W4" s="3" t="n">
-        <v>2</v>
+        <v>9</v>
       </c>
       <c r="X4" s="3" t="n">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="Y4" s="3" t="n">
         <v>5</v>
       </c>
       <c r="Z4" s="3" t="n">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="AA4" s="3" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="AB4" s="3" t="n">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="AC4" s="3" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="AD4" s="3" t="n">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="AE4" s="3" t="n">
-        <v>7</v>
+        <v>9</v>
+      </c>
+      <c r="AF4" s="3" t="n">
+        <v>10</v>
+      </c>
+      <c r="AG4" s="3" t="n">
+        <v>5</v>
+      </c>
+      <c r="AH4" s="3" t="n">
+        <v>4</v>
+      </c>
+      <c r="AI4" s="3" t="n">
+        <v>6</v>
       </c>
     </row>
     <row r="5" ht="20" customHeight="1">
@@ -938,19 +1017,19 @@
         <v>1</v>
       </c>
       <c r="C5" s="3" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D5" s="3" t="n">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="E5" s="3" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F5" s="3" t="n">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="G5" s="3" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="H5" s="3" t="n">
         <v>0</v>
@@ -959,70 +1038,82 @@
         <v>1</v>
       </c>
       <c r="J5" s="3" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="K5" s="3" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="L5" s="3" t="n">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="M5" s="3" t="n">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="N5" s="3" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="O5" s="3" t="n">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="P5" s="3" t="n">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="Q5" s="3" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="R5" s="3" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="S5" s="3" t="n">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="T5" s="3" t="n">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="U5" s="3" t="n">
         <v>7</v>
       </c>
       <c r="V5" s="3" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="W5" s="3" t="n">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="X5" s="3" t="n">
-        <v>2</v>
+        <v>9</v>
       </c>
       <c r="Y5" s="3" t="n">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="Z5" s="3" t="n">
         <v>5</v>
       </c>
       <c r="AA5" s="3" t="n">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="AB5" s="3" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="AC5" s="3" t="n">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="AD5" s="3" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="AE5" s="3" t="n">
-        <v>6</v>
+        <v>8</v>
+      </c>
+      <c r="AF5" s="3" t="n">
+        <v>9</v>
+      </c>
+      <c r="AG5" s="3" t="n">
+        <v>10</v>
+      </c>
+      <c r="AH5" s="3" t="n">
+        <v>5</v>
+      </c>
+      <c r="AI5" s="3" t="n">
+        <v>4</v>
       </c>
     </row>
     <row r="6" ht="20" customHeight="1">
@@ -1031,79 +1122,107 @@
           <t>First Aid</t>
         </is>
       </c>
-      <c r="B6" s="3" t="inlineStr"/>
-      <c r="C6" s="3" t="inlineStr"/>
-      <c r="D6" s="3" t="inlineStr"/>
-      <c r="E6" s="3" t="inlineStr"/>
-      <c r="F6" s="3" t="inlineStr"/>
-      <c r="G6" s="3" t="inlineStr"/>
-      <c r="H6" s="3" t="inlineStr"/>
-      <c r="I6" s="3" t="inlineStr"/>
+      <c r="B6" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="C6" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="D6" s="3" t="n">
+        <v>3</v>
+      </c>
+      <c r="E6" s="3" t="n">
+        <v>5</v>
+      </c>
+      <c r="F6" s="3" t="n">
+        <v>2</v>
+      </c>
+      <c r="G6" s="3" t="n">
+        <v>6</v>
+      </c>
+      <c r="H6" s="3" t="n">
+        <v>4</v>
+      </c>
+      <c r="I6" s="3" t="n">
+        <v>0</v>
+      </c>
       <c r="J6" s="3" t="n">
         <v>1</v>
       </c>
       <c r="K6" s="3" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="L6" s="3" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="M6" s="3" t="n">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="N6" s="3" t="n">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="O6" s="3" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="P6" s="3" t="n">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="Q6" s="3" t="n">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="R6" s="3" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="S6" s="3" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="T6" s="3" t="n">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="U6" s="3" t="n">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="V6" s="3" t="n">
         <v>7</v>
       </c>
       <c r="W6" s="3" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="X6" s="3" t="n">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="Y6" s="3" t="n">
-        <v>2</v>
+        <v>9</v>
       </c>
       <c r="Z6" s="3" t="n">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="AA6" s="3" t="n">
         <v>5</v>
       </c>
       <c r="AB6" s="3" t="n">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="AC6" s="3" t="n">
-        <v>4</v>
-      </c>
-      <c r="AD6" s="4" t="n">
-        <v>5</v>
+        <v>6</v>
+      </c>
+      <c r="AD6" s="3" t="n">
+        <v>7</v>
       </c>
       <c r="AE6" s="3" t="n">
-        <v>2</v>
+        <v>0</v>
+      </c>
+      <c r="AF6" s="3" t="n">
+        <v>8</v>
+      </c>
+      <c r="AG6" s="3" t="n">
+        <v>9</v>
+      </c>
+      <c r="AH6" s="3" t="n">
+        <v>10</v>
+      </c>
+      <c r="AI6" s="3" t="n">
+        <v>5</v>
       </c>
     </row>
     <row r="7" ht="20" customHeight="1">
@@ -1112,40 +1231,108 @@
           <t>Slide</t>
         </is>
       </c>
-      <c r="B7" s="3" t="inlineStr"/>
-      <c r="C7" s="3" t="inlineStr"/>
-      <c r="D7" s="3" t="inlineStr"/>
-      <c r="E7" s="3" t="inlineStr"/>
-      <c r="F7" s="3" t="inlineStr"/>
-      <c r="G7" s="3" t="inlineStr"/>
-      <c r="H7" s="3" t="inlineStr"/>
-      <c r="I7" s="3" t="inlineStr"/>
-      <c r="J7" s="3" t="inlineStr"/>
-      <c r="K7" s="3" t="inlineStr"/>
-      <c r="L7" s="3" t="inlineStr"/>
-      <c r="M7" s="3" t="inlineStr"/>
+      <c r="B7" s="3" t="n">
+        <v>4</v>
+      </c>
+      <c r="C7" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="D7" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="E7" s="3" t="n">
+        <v>3</v>
+      </c>
+      <c r="F7" s="3" t="n">
+        <v>5</v>
+      </c>
+      <c r="G7" s="3" t="n">
+        <v>2</v>
+      </c>
+      <c r="H7" s="3" t="n">
+        <v>6</v>
+      </c>
+      <c r="I7" s="3" t="n">
+        <v>4</v>
+      </c>
+      <c r="J7" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="K7" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="L7" s="3" t="n">
+        <v>3</v>
+      </c>
+      <c r="M7" s="3" t="n">
+        <v>5</v>
+      </c>
       <c r="N7" s="3" t="n">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="O7" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="P7" s="3" t="inlineStr"/>
-      <c r="Q7" s="3" t="inlineStr"/>
-      <c r="R7" s="3" t="inlineStr"/>
-      <c r="S7" s="3" t="inlineStr"/>
-      <c r="T7" s="3" t="inlineStr"/>
-      <c r="U7" s="3" t="inlineStr"/>
-      <c r="V7" s="3" t="inlineStr"/>
-      <c r="W7" s="3" t="inlineStr"/>
-      <c r="X7" s="3" t="inlineStr"/>
-      <c r="Y7" s="3" t="inlineStr"/>
-      <c r="Z7" s="3" t="inlineStr"/>
-      <c r="AA7" s="3" t="inlineStr"/>
-      <c r="AB7" s="3" t="inlineStr"/>
-      <c r="AC7" s="3" t="inlineStr"/>
-      <c r="AD7" s="3" t="inlineStr"/>
-      <c r="AE7" s="3" t="inlineStr"/>
+        <v>7</v>
+      </c>
+      <c r="P7" s="3" t="n">
+        <v>6</v>
+      </c>
+      <c r="Q7" s="3" t="n">
+        <v>8</v>
+      </c>
+      <c r="R7" s="3" t="n">
+        <v>9</v>
+      </c>
+      <c r="S7" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="T7" s="3" t="n">
+        <v>3</v>
+      </c>
+      <c r="U7" s="3" t="n">
+        <v>4</v>
+      </c>
+      <c r="V7" s="3" t="n">
+        <v>6</v>
+      </c>
+      <c r="W7" s="3" t="n">
+        <v>7</v>
+      </c>
+      <c r="X7" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y7" s="3" t="n">
+        <v>8</v>
+      </c>
+      <c r="Z7" s="3" t="n">
+        <v>9</v>
+      </c>
+      <c r="AA7" s="3" t="n">
+        <v>10</v>
+      </c>
+      <c r="AB7" s="3" t="n">
+        <v>5</v>
+      </c>
+      <c r="AC7" s="3" t="n">
+        <v>4</v>
+      </c>
+      <c r="AD7" s="3" t="n">
+        <v>6</v>
+      </c>
+      <c r="AE7" s="3" t="n">
+        <v>7</v>
+      </c>
+      <c r="AF7" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="AG7" s="3" t="n">
+        <v>8</v>
+      </c>
+      <c r="AH7" s="3" t="n">
+        <v>9</v>
+      </c>
+      <c r="AI7" s="3" t="n">
+        <v>10</v>
+      </c>
     </row>
     <row r="8" ht="20" customHeight="1">
       <c r="A8" s="2" t="inlineStr">
@@ -1183,6 +1370,10 @@
       <c r="AC8" s="3" t="inlineStr"/>
       <c r="AD8" s="3" t="inlineStr"/>
       <c r="AE8" s="3" t="inlineStr"/>
+      <c r="AF8" s="3" t="inlineStr"/>
+      <c r="AG8" s="3" t="inlineStr"/>
+      <c r="AH8" s="3" t="inlineStr"/>
+      <c r="AI8" s="3" t="inlineStr"/>
     </row>
     <row r="9" ht="20" customHeight="1">
       <c r="A9" s="2" t="inlineStr">
@@ -1220,6 +1411,10 @@
       <c r="AC9" s="3" t="inlineStr"/>
       <c r="AD9" s="3" t="inlineStr"/>
       <c r="AE9" s="3" t="inlineStr"/>
+      <c r="AF9" s="3" t="inlineStr"/>
+      <c r="AG9" s="3" t="inlineStr"/>
+      <c r="AH9" s="3" t="inlineStr"/>
+      <c r="AI9" s="3" t="inlineStr"/>
     </row>
     <row r="10" ht="20" customHeight="1">
       <c r="A10" s="2" t="inlineStr">
@@ -1228,94 +1423,106 @@
         </is>
       </c>
       <c r="B10" s="3" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="C10" s="3" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="D10" s="3" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="E10" s="3" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F10" s="3" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="G10" s="3" t="n">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="H10" s="3" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="I10" s="3" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="J10" s="3" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="K10" s="3" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L10" s="3" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="M10" s="3" t="n">
         <v>3</v>
       </c>
       <c r="N10" s="3" t="n">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="O10" s="3" t="n">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="P10" s="3" t="n">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="Q10" s="3" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="R10" s="3" t="n">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="S10" s="3" t="n">
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="T10" s="3" t="n">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="U10" s="3" t="n">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="V10" s="3" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="W10" s="3" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="X10" s="3" t="n">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="Y10" s="3" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="Z10" s="3" t="n">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="AA10" s="3" t="n">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="AB10" s="3" t="n">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="AC10" s="3" t="n">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="AD10" s="3" t="n">
         <v>4</v>
       </c>
       <c r="AE10" s="3" t="n">
-        <v>5</v>
+        <v>6</v>
+      </c>
+      <c r="AF10" s="3" t="n">
+        <v>7</v>
+      </c>
+      <c r="AG10" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="AH10" s="3" t="n">
+        <v>8</v>
+      </c>
+      <c r="AI10" s="3" t="n">
+        <v>9</v>
       </c>
     </row>
     <row r="11" ht="20" customHeight="1">
@@ -1332,28 +1539,80 @@
       <c r="G11" s="3" t="inlineStr"/>
       <c r="H11" s="3" t="inlineStr"/>
       <c r="I11" s="3" t="inlineStr"/>
-      <c r="J11" s="3" t="inlineStr"/>
-      <c r="K11" s="3" t="inlineStr"/>
-      <c r="L11" s="3" t="inlineStr"/>
-      <c r="M11" s="3" t="inlineStr"/>
-      <c r="N11" s="3" t="inlineStr"/>
-      <c r="O11" s="3" t="inlineStr"/>
-      <c r="P11" s="3" t="inlineStr"/>
-      <c r="Q11" s="3" t="inlineStr"/>
-      <c r="R11" s="3" t="inlineStr"/>
-      <c r="S11" s="3" t="inlineStr"/>
-      <c r="T11" s="3" t="inlineStr"/>
-      <c r="U11" s="3" t="inlineStr"/>
-      <c r="V11" s="3" t="inlineStr"/>
-      <c r="W11" s="3" t="inlineStr"/>
-      <c r="X11" s="3" t="inlineStr"/>
-      <c r="Y11" s="3" t="inlineStr"/>
-      <c r="Z11" s="3" t="inlineStr"/>
-      <c r="AA11" s="3" t="inlineStr"/>
-      <c r="AB11" s="3" t="inlineStr"/>
-      <c r="AC11" s="3" t="inlineStr"/>
-      <c r="AD11" s="3" t="inlineStr"/>
-      <c r="AE11" s="3" t="inlineStr"/>
+      <c r="J11" s="3" t="n">
+        <v>6</v>
+      </c>
+      <c r="K11" s="3" t="n">
+        <v>4</v>
+      </c>
+      <c r="L11" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="M11" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="N11" s="3" t="n">
+        <v>3</v>
+      </c>
+      <c r="O11" s="3" t="n">
+        <v>5</v>
+      </c>
+      <c r="P11" s="3" t="n">
+        <v>2</v>
+      </c>
+      <c r="Q11" s="3" t="n">
+        <v>7</v>
+      </c>
+      <c r="R11" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="S11" s="3" t="n">
+        <v>8</v>
+      </c>
+      <c r="T11" s="3" t="n">
+        <v>9</v>
+      </c>
+      <c r="U11" s="3" t="n">
+        <v>10</v>
+      </c>
+      <c r="V11" s="3" t="n">
+        <v>5</v>
+      </c>
+      <c r="W11" s="3" t="n">
+        <v>4</v>
+      </c>
+      <c r="X11" s="3" t="n">
+        <v>6</v>
+      </c>
+      <c r="Y11" s="3" t="n">
+        <v>7</v>
+      </c>
+      <c r="Z11" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA11" s="3" t="n">
+        <v>8</v>
+      </c>
+      <c r="AB11" s="3" t="n">
+        <v>9</v>
+      </c>
+      <c r="AC11" s="3" t="n">
+        <v>10</v>
+      </c>
+      <c r="AD11" s="3" t="n">
+        <v>5</v>
+      </c>
+      <c r="AE11" s="3" t="n">
+        <v>4</v>
+      </c>
+      <c r="AF11" s="3" t="n">
+        <v>6</v>
+      </c>
+      <c r="AG11" s="3" t="n">
+        <v>7</v>
+      </c>
+      <c r="AH11" s="3" t="inlineStr"/>
+      <c r="AI11" s="3" t="inlineStr"/>
     </row>
     <row r="12" ht="20" customHeight="1">
       <c r="A12" s="2" t="inlineStr">
@@ -1391,6 +1650,10 @@
       <c r="AC12" s="3" t="inlineStr"/>
       <c r="AD12" s="3" t="inlineStr"/>
       <c r="AE12" s="3" t="inlineStr"/>
+      <c r="AF12" s="3" t="inlineStr"/>
+      <c r="AG12" s="3" t="inlineStr"/>
+      <c r="AH12" s="3" t="inlineStr"/>
+      <c r="AI12" s="3" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>